<commit_message>
16.04.19 Today Sales Last Updated 09:00 Pm
</commit_message>
<xml_diff>
--- a/Daily requisition analysis of Tulip -2, Bagha..xlsx
+++ b/Daily requisition analysis of Tulip -2, Bagha..xlsx
@@ -10,14 +10,14 @@
     <sheet name="Daily Requisition" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$129</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="159">
   <si>
     <t>Model Name</t>
   </si>
@@ -28,499 +28,472 @@
     <t>BL20</t>
   </si>
   <si>
-    <t>BL60</t>
-  </si>
-  <si>
     <t>BL80</t>
   </si>
   <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>D68</t>
+  </si>
+  <si>
+    <t>D75</t>
+  </si>
+  <si>
+    <t>D91</t>
+  </si>
+  <si>
+    <t>D101</t>
+  </si>
+  <si>
+    <t>D105</t>
+  </si>
+  <si>
+    <t>D140</t>
+  </si>
+  <si>
+    <t>D150</t>
+  </si>
+  <si>
+    <t>E30</t>
+  </si>
+  <si>
+    <t>E58</t>
+  </si>
+  <si>
+    <t>E79</t>
+  </si>
+  <si>
+    <t>E80</t>
+  </si>
+  <si>
+    <t>E82</t>
+  </si>
+  <si>
+    <t>i10</t>
+  </si>
+  <si>
+    <t>i21</t>
+  </si>
+  <si>
+    <t>i50</t>
+  </si>
+  <si>
+    <t>i60</t>
+  </si>
+  <si>
+    <t>i90</t>
+  </si>
+  <si>
+    <t>L16</t>
+  </si>
+  <si>
+    <t>L23</t>
+  </si>
+  <si>
+    <t>L24</t>
+  </si>
+  <si>
+    <t>L25</t>
+  </si>
+  <si>
+    <t>L26</t>
+  </si>
+  <si>
+    <t>L50</t>
+  </si>
+  <si>
+    <t>L55</t>
+  </si>
+  <si>
+    <t>L65</t>
+  </si>
+  <si>
+    <t>L100</t>
+  </si>
+  <si>
+    <t>L150</t>
+  </si>
+  <si>
+    <t>L200</t>
+  </si>
+  <si>
+    <t>L300</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P7 Pro</t>
+  </si>
+  <si>
+    <t>P8 Pro</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P9+</t>
+  </si>
+  <si>
+    <t>P9_2GB</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R100_2GB</t>
+  </si>
+  <si>
+    <t>R100_3GB</t>
+  </si>
+  <si>
+    <t>S50</t>
+  </si>
+  <si>
+    <t>T85</t>
+  </si>
+  <si>
+    <t>T105</t>
+  </si>
+  <si>
+    <t>T110</t>
+  </si>
+  <si>
+    <t>T160</t>
+  </si>
+  <si>
+    <t>T200</t>
+  </si>
+  <si>
+    <t>V20</t>
+  </si>
+  <si>
+    <t>V32</t>
+  </si>
+  <si>
+    <t>V34</t>
+  </si>
+  <si>
+    <t>V42</t>
+  </si>
+  <si>
+    <t>V46(C)</t>
+  </si>
+  <si>
+    <t>V47</t>
+  </si>
+  <si>
+    <t>V65</t>
+  </si>
+  <si>
+    <t>V75m</t>
+  </si>
+  <si>
+    <t>V75m_2GB</t>
+  </si>
+  <si>
+    <t>V90</t>
+  </si>
+  <si>
+    <t>V95</t>
+  </si>
+  <si>
+    <t>V110</t>
+  </si>
+  <si>
+    <t>V120</t>
+  </si>
+  <si>
+    <t>Z9</t>
+  </si>
+  <si>
+    <t>Z10</t>
+  </si>
+  <si>
+    <t>Today's Order Quantity</t>
+  </si>
+  <si>
+    <t>Order Value</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Dealer Price</t>
+  </si>
+  <si>
+    <t>Total=</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>SCB</t>
+  </si>
+  <si>
+    <t>BRAC</t>
+  </si>
+  <si>
+    <t>DBBL</t>
+  </si>
+  <si>
+    <t>IBBL</t>
+  </si>
+  <si>
+    <t>UBL</t>
+  </si>
+  <si>
+    <t>Payment Details</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>EDISON GROUP_SYMPHONY MOBILE</t>
+  </si>
+  <si>
+    <t>B12i</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Sym Tab 25</t>
+  </si>
+  <si>
+    <t>Sym Tab 60</t>
+  </si>
+  <si>
+    <t>White gold</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>V130</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>D38</t>
+  </si>
+  <si>
+    <t>i70</t>
+  </si>
+  <si>
+    <t>BL70</t>
+  </si>
+  <si>
+    <t>L120</t>
+  </si>
+  <si>
+    <t>BL100</t>
+  </si>
+  <si>
+    <t>i100</t>
+  </si>
+  <si>
+    <t>Gray+Blue</t>
+  </si>
+  <si>
+    <t>i90_2GB</t>
+  </si>
+  <si>
+    <t>D39</t>
+  </si>
+  <si>
+    <t>BL75</t>
+  </si>
+  <si>
+    <t>Must be Black</t>
+  </si>
+  <si>
+    <t>BL110</t>
+  </si>
+  <si>
+    <t>V78</t>
+  </si>
+  <si>
+    <t>D52j</t>
+  </si>
+  <si>
+    <t>D69</t>
+  </si>
+  <si>
+    <t>L60</t>
+  </si>
+  <si>
+    <t>V140</t>
+  </si>
+  <si>
+    <t>V92</t>
+  </si>
+  <si>
+    <t>V96</t>
+  </si>
+  <si>
+    <t>i75</t>
+  </si>
+  <si>
+    <t>V44</t>
+  </si>
+  <si>
+    <t>V135</t>
+  </si>
+  <si>
+    <t>i15</t>
+  </si>
+  <si>
+    <t>i120</t>
+  </si>
+  <si>
+    <t>V150</t>
+  </si>
+  <si>
+    <t>helio S5</t>
+  </si>
+  <si>
+    <t>helio S60</t>
+  </si>
+  <si>
+    <t>helio S10</t>
+  </si>
+  <si>
+    <t>helio S2</t>
+  </si>
+  <si>
+    <t>Black+ Blue</t>
+  </si>
+  <si>
+    <t>V98</t>
+  </si>
+  <si>
+    <t>V145</t>
+  </si>
+  <si>
+    <t>BL95</t>
+  </si>
+  <si>
+    <t>V155</t>
+  </si>
+  <si>
+    <t>T130</t>
+  </si>
+  <si>
+    <t>E90</t>
+  </si>
+  <si>
+    <t>V94</t>
+  </si>
+  <si>
+    <t>V75_SKD</t>
+  </si>
+  <si>
+    <t>Must be Blue</t>
+  </si>
+  <si>
+    <t>T140</t>
+  </si>
+  <si>
+    <t>B17i</t>
+  </si>
+  <si>
+    <t>i10+_SKD</t>
+  </si>
+  <si>
+    <t>V48</t>
+  </si>
+  <si>
+    <t>D40</t>
+  </si>
+  <si>
+    <t>White Rose Gold</t>
+  </si>
+  <si>
+    <t>D38i</t>
+  </si>
+  <si>
+    <t>Gold &amp; Black</t>
+  </si>
+  <si>
+    <t>V97</t>
+  </si>
+  <si>
+    <t>i95</t>
+  </si>
+  <si>
+    <t>Blue Black, Gold, Black, Red Black</t>
+  </si>
+  <si>
+    <t>V142</t>
+  </si>
+  <si>
+    <t>Gold/ Black</t>
+  </si>
+  <si>
+    <t>Zone: Rajshahi</t>
+  </si>
+  <si>
+    <t>i110_SKD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue Black, Gold, Black, </t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Black,White</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>DEL-Tulip -2</t>
+  </si>
+  <si>
+    <t>Dealer ID:</t>
+  </si>
+  <si>
+    <t>Daily Requisition for Tulip -2</t>
+  </si>
+  <si>
+    <t>Black_Gold</t>
+  </si>
+  <si>
+    <t>Darkblue</t>
+  </si>
+  <si>
+    <t>D52J</t>
+  </si>
+  <si>
+    <t>D54J</t>
+  </si>
+  <si>
+    <t>Black_Blue</t>
+  </si>
+  <si>
     <t>BL90</t>
   </si>
   <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>D19</t>
-  </si>
-  <si>
-    <t>D22</t>
-  </si>
-  <si>
-    <t>D68</t>
-  </si>
-  <si>
-    <t>D75</t>
-  </si>
-  <si>
-    <t>D91</t>
-  </si>
-  <si>
-    <t>D101</t>
-  </si>
-  <si>
-    <t>D105</t>
-  </si>
-  <si>
-    <t>D140</t>
-  </si>
-  <si>
-    <t>D150</t>
-  </si>
-  <si>
-    <t>E30</t>
-  </si>
-  <si>
-    <t>E58</t>
-  </si>
-  <si>
-    <t>E79</t>
-  </si>
-  <si>
-    <t>E80</t>
-  </si>
-  <si>
-    <t>E82</t>
-  </si>
-  <si>
-    <t>i10</t>
-  </si>
-  <si>
-    <t>i21</t>
-  </si>
-  <si>
-    <t>i50</t>
-  </si>
-  <si>
-    <t>i60</t>
-  </si>
-  <si>
-    <t>i90</t>
-  </si>
-  <si>
-    <t>L16</t>
-  </si>
-  <si>
-    <t>L23</t>
-  </si>
-  <si>
-    <t>L24</t>
-  </si>
-  <si>
-    <t>L25</t>
-  </si>
-  <si>
-    <t>L26</t>
-  </si>
-  <si>
-    <t>L50</t>
-  </si>
-  <si>
-    <t>L55</t>
-  </si>
-  <si>
-    <t>L65</t>
-  </si>
-  <si>
-    <t>L100</t>
-  </si>
-  <si>
-    <t>L150</t>
-  </si>
-  <si>
-    <t>L200</t>
-  </si>
-  <si>
-    <t>L300</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P7 Pro</t>
-  </si>
-  <si>
-    <t>P8 Pro</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>P9+</t>
-  </si>
-  <si>
-    <t>P9_2GB</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R100_2GB</t>
-  </si>
-  <si>
-    <t>R100_3GB</t>
-  </si>
-  <si>
-    <t>S50</t>
-  </si>
-  <si>
-    <t>T85</t>
-  </si>
-  <si>
-    <t>T105</t>
-  </si>
-  <si>
-    <t>T110</t>
-  </si>
-  <si>
-    <t>T160</t>
-  </si>
-  <si>
-    <t>T200</t>
-  </si>
-  <si>
-    <t>V20</t>
-  </si>
-  <si>
-    <t>V32</t>
-  </si>
-  <si>
-    <t>V34</t>
-  </si>
-  <si>
-    <t>V42</t>
-  </si>
-  <si>
-    <t>V46(C)</t>
-  </si>
-  <si>
-    <t>V47</t>
-  </si>
-  <si>
-    <t>V65</t>
-  </si>
-  <si>
-    <t>V75m</t>
-  </si>
-  <si>
-    <t>V75m_2GB</t>
-  </si>
-  <si>
-    <t>V90</t>
-  </si>
-  <si>
-    <t>V95</t>
-  </si>
-  <si>
-    <t>V110</t>
-  </si>
-  <si>
-    <t>V120</t>
-  </si>
-  <si>
-    <t>Z9</t>
-  </si>
-  <si>
-    <t>Z10</t>
-  </si>
-  <si>
-    <t>Today's Order Quantity</t>
-  </si>
-  <si>
-    <t>Order Value</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Dealer Price</t>
-  </si>
-  <si>
-    <t>Total=</t>
-  </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>SCB</t>
-  </si>
-  <si>
-    <t>BRAC</t>
-  </si>
-  <si>
-    <t>DBBL</t>
-  </si>
-  <si>
-    <t>IBBL</t>
-  </si>
-  <si>
-    <t>UBL</t>
-  </si>
-  <si>
-    <t>Payment Details</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>EDISON GROUP_SYMPHONY MOBILE</t>
-  </si>
-  <si>
-    <t>B12i</t>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>Sym Tab 25</t>
-  </si>
-  <si>
-    <t>Sym Tab 60</t>
-  </si>
-  <si>
-    <t>White gold</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>V130</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>D38</t>
-  </si>
-  <si>
-    <t>i70</t>
-  </si>
-  <si>
-    <t>BL70</t>
-  </si>
-  <si>
-    <t>L120</t>
-  </si>
-  <si>
-    <t>BL100</t>
-  </si>
-  <si>
-    <t>i100</t>
-  </si>
-  <si>
-    <t>Gray+Blue</t>
-  </si>
-  <si>
-    <t>i90_2GB</t>
-  </si>
-  <si>
-    <t>D39</t>
-  </si>
-  <si>
-    <t>B22</t>
-  </si>
-  <si>
-    <t>BL75</t>
-  </si>
-  <si>
-    <t>B21</t>
-  </si>
-  <si>
-    <t>Must be Black</t>
-  </si>
-  <si>
-    <t>BL110</t>
-  </si>
-  <si>
-    <t>V78</t>
-  </si>
-  <si>
-    <t>D52j</t>
-  </si>
-  <si>
-    <t>D69</t>
-  </si>
-  <si>
-    <t>L60</t>
-  </si>
-  <si>
-    <t>V140</t>
-  </si>
-  <si>
-    <t>V92</t>
-  </si>
-  <si>
-    <t>V96</t>
-  </si>
-  <si>
-    <t>i75</t>
-  </si>
-  <si>
-    <t>V44</t>
-  </si>
-  <si>
-    <t>B23</t>
-  </si>
-  <si>
-    <t>V135</t>
-  </si>
-  <si>
-    <t>i15</t>
-  </si>
-  <si>
-    <t>i120</t>
-  </si>
-  <si>
-    <t>V150</t>
-  </si>
-  <si>
-    <t>helio S5</t>
-  </si>
-  <si>
-    <t>helio S60</t>
-  </si>
-  <si>
-    <t>helio S10</t>
-  </si>
-  <si>
-    <t>helio S2</t>
-  </si>
-  <si>
-    <t>Black+ Blue</t>
-  </si>
-  <si>
-    <t>V98</t>
-  </si>
-  <si>
-    <t>V145</t>
-  </si>
-  <si>
-    <t>BL95</t>
-  </si>
-  <si>
-    <t>V155</t>
-  </si>
-  <si>
-    <t>T130</t>
-  </si>
-  <si>
-    <t>E90</t>
-  </si>
-  <si>
-    <t>V94</t>
-  </si>
-  <si>
-    <t>V75_SKD</t>
-  </si>
-  <si>
-    <t>Must be Blue</t>
-  </si>
-  <si>
-    <t>T140</t>
-  </si>
-  <si>
-    <t>B17i</t>
-  </si>
-  <si>
-    <t>i10+_SKD</t>
-  </si>
-  <si>
-    <t>V48</t>
-  </si>
-  <si>
-    <t>D40</t>
-  </si>
-  <si>
-    <t>White Rose Gold</t>
-  </si>
-  <si>
-    <t>D38i</t>
-  </si>
-  <si>
-    <t>Gold &amp; Black</t>
-  </si>
-  <si>
-    <t>V97</t>
-  </si>
-  <si>
-    <t>i95</t>
-  </si>
-  <si>
-    <t>Blue Black, Gold, Black, Red Black</t>
-  </si>
-  <si>
-    <t>V142</t>
-  </si>
-  <si>
-    <t>Gold/ Black</t>
-  </si>
-  <si>
-    <t>Zone: Rajshahi</t>
-  </si>
-  <si>
-    <t>i110_SKD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blue Black, Gold, Black, </t>
-  </si>
-  <si>
-    <t>Mixed</t>
-  </si>
-  <si>
-    <t>Blue, Gold,  Red</t>
-  </si>
-  <si>
-    <t>Mixed,White</t>
-  </si>
-  <si>
-    <t>Black,White</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>DEL-Tulip -2</t>
-  </si>
-  <si>
-    <t>Dealer ID:</t>
-  </si>
-  <si>
-    <t>Daily Requisition for Tulip -2</t>
-  </si>
-  <si>
-    <t>13.04.19</t>
-  </si>
-  <si>
-    <t>b23</t>
-  </si>
-  <si>
-    <t>bl60</t>
-  </si>
-  <si>
-    <t>d52j</t>
-  </si>
-  <si>
-    <t>l110</t>
-  </si>
-  <si>
-    <t>l23i</t>
-  </si>
-  <si>
-    <t>Mixed/Black</t>
-  </si>
-  <si>
-    <t>v155</t>
-  </si>
-  <si>
-    <t>v98</t>
-  </si>
-  <si>
-    <t>v142</t>
+    <t>16.04.19</t>
+  </si>
+  <si>
+    <t>Yellow_Black</t>
   </si>
 </sst>
 </file>
@@ -533,7 +506,7 @@
     <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,13 +559,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -744,7 +710,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -828,6 +794,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -851,18 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1171,13 +1131,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E136" sqref="E136"/>
+      <selection pane="bottomRight" activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1191,38 +1151,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="12.75">
-      <c r="A1" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="A1" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" ht="12.75">
-      <c r="A2" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="A2" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="12.75">
       <c r="A3" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1230,21 +1190,21 @@
         <v>0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" hidden="1">
       <c r="A5" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="12">
         <v>779.95</v>
@@ -1255,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" hidden="1">
@@ -1267,14 +1227,14 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="13">
-        <f t="shared" ref="D6:D95" si="0">C6*B6</f>
+        <f t="shared" ref="D6:D89" si="0">C6*B6</f>
         <v>0</v>
       </c>
       <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" ht="15" hidden="1">
       <c r="A7" s="11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B7" s="12">
         <v>789.97</v>
@@ -1285,57 +1245,59 @@
         <v>0</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="A8" s="11" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="B8" s="12">
-        <v>779.95</v>
+        <v>901.24749999999995</v>
       </c>
       <c r="C8" s="11">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D8" s="13">
-        <f t="shared" si="0"/>
-        <v>46797</v>
-      </c>
-      <c r="E8" s="11"/>
+        <f>SUM(B8*C8)</f>
+        <v>18024.949999999997</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="11" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="B9" s="12">
-        <v>774.93</v>
+        <v>858.14</v>
       </c>
       <c r="C9" s="11">
         <v>20</v>
       </c>
       <c r="D9" s="13">
         <f t="shared" si="0"/>
-        <v>15498.599999999999</v>
-      </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" ht="15">
+        <v>17162.8</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" hidden="1">
       <c r="A10" s="11" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B10" s="12">
-        <v>769.92</v>
-      </c>
-      <c r="C10" s="11">
-        <v>20</v>
-      </c>
+        <v>946.36</v>
+      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="13">
         <f t="shared" si="0"/>
-        <v>15398.4</v>
+        <v>0</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" hidden="1">
@@ -1352,27 +1314,25 @@
       </c>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A12" s="14" t="s">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="B12" s="15">
-        <v>896.23500000000001</v>
-      </c>
-      <c r="C12" s="11">
-        <v>20</v>
-      </c>
+        <v>1258.1375</v>
+      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>17924.7</v>
+        <v>0</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" hidden="1">
       <c r="A13" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="12">
         <v>887.21</v>
@@ -1386,7 +1346,7 @@
     </row>
     <row r="14" spans="1:5" ht="15" hidden="1">
       <c r="A14" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B14" s="12">
         <v>868.17</v>
@@ -1400,7 +1360,7 @@
     </row>
     <row r="15" spans="1:5" ht="15" hidden="1">
       <c r="A15" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="12">
         <v>877.1875</v>
@@ -1414,43 +1374,41 @@
     </row>
     <row r="16" spans="1:5" ht="15">
       <c r="A16" s="11" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="B16" s="12">
-        <v>901.24749999999995</v>
+        <v>1238.0875000000001</v>
       </c>
       <c r="C16" s="11">
         <v>20</v>
       </c>
       <c r="D16" s="13">
         <f t="shared" si="0"/>
-        <v>18024.949999999997</v>
+        <v>24761.75</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" hidden="1">
       <c r="A17" s="11" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="B17" s="12">
-        <v>858.14</v>
-      </c>
-      <c r="C17" s="11">
-        <v>20</v>
-      </c>
+        <v>975.4325</v>
+      </c>
+      <c r="C17" s="11"/>
       <c r="D17" s="13">
         <f t="shared" si="0"/>
-        <v>17162.8</v>
+        <v>0</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A18" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B18" s="15">
         <v>985.46</v>
@@ -1464,7 +1422,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" hidden="1">
       <c r="A19" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B19" s="12">
         <v>946.36</v>
@@ -1478,7 +1436,7 @@
     </row>
     <row r="20" spans="1:5" ht="15" hidden="1">
       <c r="A20" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="12">
         <v>1064.655</v>
@@ -1492,7 +1450,7 @@
     </row>
     <row r="21" spans="1:5" ht="15" hidden="1">
       <c r="A21" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="12">
         <v>1430.5675000000001</v>
@@ -1503,12 +1461,12 @@
         <v>0</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" hidden="1">
       <c r="A22" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22" s="12">
         <v>1538.8375000000001</v>
@@ -1519,12 +1477,12 @@
         <v>0</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" hidden="1">
       <c r="A23" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23" s="12">
         <v>1654.125</v>
@@ -1538,7 +1496,7 @@
     </row>
     <row r="24" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A24" s="14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24" s="15">
         <v>980.44500000000005</v>
@@ -1549,12 +1507,12 @@
         <v>0</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" hidden="1">
       <c r="A25" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" s="12">
         <v>940.34500000000003</v>
@@ -1568,7 +1526,7 @@
     </row>
     <row r="26" spans="1:5" ht="15" hidden="1">
       <c r="A26" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26" s="12">
         <v>975.4325</v>
@@ -1579,12 +1537,12 @@
         <v>0</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" hidden="1">
       <c r="A27" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B27" s="12">
         <v>1258.1400000000001</v>
@@ -1596,9 +1554,9 @@
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" hidden="1" thickBot="1">
+    <row r="28" spans="1:5" ht="15" hidden="1">
       <c r="A28" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B28" s="12">
         <v>1258.1400000000001</v>
@@ -1612,7 +1570,7 @@
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A29" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B29" s="15">
         <v>975.43</v>
@@ -1623,12 +1581,12 @@
         <v>0</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A30" s="14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B30" s="15">
         <v>936.34</v>
@@ -1639,12 +1597,12 @@
         <v>0</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" hidden="1">
       <c r="A31" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" s="12">
         <v>955.38</v>
@@ -1658,7 +1616,7 @@
     </row>
     <row r="32" spans="1:5" ht="15" hidden="1">
       <c r="A32" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B32" s="12">
         <v>1014.53</v>
@@ -1672,7 +1630,7 @@
     </row>
     <row r="33" spans="1:5" ht="15" hidden="1">
       <c r="A33" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B33" s="12">
         <v>1145.8575000000001</v>
@@ -1684,25 +1642,27 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="15">
       <c r="A34" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B34" s="15">
         <v>1159.8900000000001</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="11">
+        <v>20</v>
+      </c>
       <c r="D34" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23197.800000000003</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" hidden="1">
       <c r="A35" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B35" s="12">
         <v>1264.1524999999999</v>
@@ -1713,12 +1673,12 @@
         <v>0</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" hidden="1">
       <c r="A36" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" s="12">
         <v>1165.9075</v>
@@ -1732,7 +1692,7 @@
     </row>
     <row r="37" spans="1:5" ht="15" hidden="1">
       <c r="A37" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B37" s="12">
         <v>2309.7600000000002</v>
@@ -1746,7 +1706,7 @@
     </row>
     <row r="38" spans="1:5" ht="15" hidden="1">
       <c r="A38" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B38" s="12">
         <v>2556.375</v>
@@ -1760,7 +1720,7 @@
     </row>
     <row r="39" spans="1:5" ht="15" hidden="1">
       <c r="A39" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39" s="12">
         <v>2731.8125</v>
@@ -1774,7 +1734,7 @@
     </row>
     <row r="40" spans="1:5" ht="15" hidden="1">
       <c r="A40" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B40" s="12">
         <v>2812.0124999999998</v>
@@ -1788,7 +1748,7 @@
     </row>
     <row r="41" spans="1:5" ht="15" hidden="1">
       <c r="A41" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B41" s="12">
         <v>2714.77</v>
@@ -1799,12 +1759,12 @@
         <v>0</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" hidden="1">
       <c r="A42" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B42" s="12">
         <v>2788.96</v>
@@ -1815,12 +1775,12 @@
         <v>0</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" hidden="1">
       <c r="A43" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="12">
         <v>6416</v>
@@ -1831,12 +1791,12 @@
         <v>0</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" hidden="1">
       <c r="A44" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B44" s="12">
         <v>6397.96</v>
@@ -1847,12 +1807,12 @@
         <v>0</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" hidden="1">
       <c r="A45" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B45" s="12">
         <v>6057.11</v>
@@ -1863,12 +1823,12 @@
         <v>0</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" hidden="1">
       <c r="A46" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B46" s="12">
         <v>5819.5124999999998</v>
@@ -1879,12 +1839,12 @@
         <v>0</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" hidden="1">
       <c r="A47" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B47" s="12">
         <v>6877.15</v>
@@ -1898,7 +1858,7 @@
     </row>
     <row r="48" spans="1:5" ht="15" hidden="1">
       <c r="A48" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B48" s="12">
         <v>6937.3</v>
@@ -1909,12 +1869,12 @@
         <v>0</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" hidden="1">
       <c r="A49" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B49" s="12">
         <v>7851.58</v>
@@ -1925,12 +1885,12 @@
         <v>0</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" hidden="1">
       <c r="A50" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B50" s="12">
         <v>7714.24</v>
@@ -1941,12 +1901,12 @@
         <v>0</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" hidden="1">
       <c r="A51" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B51" s="12">
         <v>8225.5125000000007</v>
@@ -1957,12 +1917,12 @@
         <v>0</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" hidden="1">
       <c r="A52" s="11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B52" s="12">
         <v>7309.23</v>
@@ -1973,12 +1933,12 @@
         <v>0</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" hidden="1">
       <c r="A53" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B53" s="12">
         <v>8877.14</v>
@@ -1989,12 +1949,12 @@
         <v>0</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" hidden="1">
       <c r="A54" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B54" s="12">
         <v>8573.3799999999992</v>
@@ -2005,12 +1965,12 @@
         <v>0</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" hidden="1">
       <c r="A55" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B55" s="12">
         <v>8967.36</v>
@@ -2021,79 +1981,77 @@
         <v>0</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15" hidden="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15">
       <c r="A56" s="11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B56" s="12">
         <v>9012.48</v>
       </c>
-      <c r="C56" s="11"/>
+      <c r="C56" s="11">
+        <v>5</v>
+      </c>
       <c r="D56" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E56" s="11"/>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" thickBot="1">
+        <v>45062.399999999994</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" hidden="1">
       <c r="A57" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B57" s="40">
-        <v>769.92</v>
-      </c>
-      <c r="C57" s="11">
-        <v>40</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B57" s="12">
+        <v>1199.9925000000001</v>
+      </c>
+      <c r="C57" s="11"/>
       <c r="D57" s="13">
-        <f t="shared" ref="D57" si="2">C57*B57</f>
-        <v>30796.799999999999</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>89</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E57" s="11"/>
     </row>
     <row r="58" spans="1:5" ht="15" hidden="1">
       <c r="A58" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B58" s="12">
-        <v>1199.9925000000001</v>
+        <v>138</v>
+      </c>
+      <c r="B58" s="31">
+        <v>7309.2275</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E58" s="11"/>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" thickBot="1">
+      <c r="E58" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15" hidden="1">
       <c r="A59" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B59" s="40">
-        <v>896.23500000000001</v>
-      </c>
-      <c r="C59" s="11">
-        <v>20</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B59" s="12">
+        <v>1423.55</v>
+      </c>
+      <c r="C59" s="11"/>
       <c r="D59" s="13">
         <f t="shared" si="0"/>
-        <v>17924.7</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>89</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E59" s="11"/>
     </row>
     <row r="60" spans="1:5" ht="15" hidden="1">
       <c r="A60" s="11" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="B60" s="12">
-        <v>1423.55</v>
+        <v>1435.58</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="13">
@@ -2104,10 +2062,10 @@
     </row>
     <row r="61" spans="1:5" ht="15" hidden="1">
       <c r="A61" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B61" s="12">
-        <v>1435.58</v>
+        <v>1551.87</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="13">
@@ -2118,10 +2076,10 @@
     </row>
     <row r="62" spans="1:5" ht="15" hidden="1">
       <c r="A62" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B62" s="12">
-        <v>1551.87</v>
+        <v>1695.2275</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="13">
@@ -2132,10 +2090,10 @@
     </row>
     <row r="63" spans="1:5" ht="15" hidden="1">
       <c r="A63" s="11" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B63" s="12">
-        <v>1695.2275</v>
+        <v>1067.6624999999999</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="13">
@@ -2146,42 +2104,40 @@
     </row>
     <row r="64" spans="1:5" ht="15" hidden="1">
       <c r="A64" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="12">
-        <v>1067.6624999999999</v>
+        <v>140</v>
+      </c>
+      <c r="B64" s="31">
+        <v>5310.2425000000003</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E64" s="11"/>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1">
+      <c r="E64" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" hidden="1">
       <c r="A65" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="40">
-        <v>1258.1375</v>
-      </c>
-      <c r="C65" s="11">
-        <v>60</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B65" s="12">
+        <v>1106.76</v>
+      </c>
+      <c r="C65" s="11"/>
       <c r="D65" s="13">
         <f t="shared" si="0"/>
-        <v>75488.25</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>164</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E65" s="11"/>
     </row>
     <row r="66" spans="1:5" ht="15" hidden="1">
       <c r="A66" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" s="12">
-        <v>1106.76</v>
+        <v>1145.8575000000001</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="13">
@@ -2190,44 +2146,42 @@
       </c>
       <c r="E66" s="11"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1">
+    <row r="67" spans="1:5" ht="15" hidden="1">
       <c r="A67" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B67" s="40">
-        <v>6937.3</v>
-      </c>
-      <c r="C67" s="11">
-        <v>5</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B67" s="12">
+        <v>1135.8325</v>
+      </c>
+      <c r="C67" s="11"/>
       <c r="D67" s="13">
         <f t="shared" si="0"/>
-        <v>34686.5</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>150</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E67" s="11"/>
     </row>
     <row r="68" spans="1:5" ht="15" hidden="1">
       <c r="A68" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" s="12">
-        <v>1145.8575000000001</v>
+        <v>137</v>
+      </c>
+      <c r="B68" s="31">
+        <v>4165.3874999999998</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E68" s="11"/>
+      <c r="E68" s="11" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="15" hidden="1">
       <c r="A69" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B69" s="12">
-        <v>1135.8325</v>
+        <v>1174.93</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="13">
@@ -2236,30 +2190,26 @@
       </c>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" thickBot="1">
+    <row r="70" spans="1:5" ht="15" hidden="1">
       <c r="A70" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B70" s="40">
-        <v>7722.2574999999997</v>
-      </c>
-      <c r="C70" s="11">
-        <v>5</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B70" s="12">
+        <v>1273.175</v>
+      </c>
+      <c r="C70" s="11"/>
       <c r="D70" s="13">
         <f t="shared" si="0"/>
-        <v>38611.287499999999</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>89</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E70" s="11"/>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1">
       <c r="A71" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B71" s="12">
-        <v>1174.93</v>
+        <v>1077.6875</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="13">
@@ -2268,30 +2218,26 @@
       </c>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A72" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="B72" s="40">
-        <v>1189.9675</v>
-      </c>
-      <c r="C72" s="11">
-        <v>20</v>
-      </c>
+    <row r="72" spans="1:5" ht="15" hidden="1">
+      <c r="A72" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B72" s="12">
+        <v>1101.75</v>
+      </c>
+      <c r="C72" s="11"/>
       <c r="D72" s="13">
         <f t="shared" si="0"/>
-        <v>23799.35</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>141</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E72" s="11"/>
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1">
       <c r="A73" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B73" s="12">
-        <v>1273.175</v>
+        <v>1303.25</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="13">
@@ -2300,30 +2246,26 @@
       </c>
       <c r="E73" s="11"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" thickBot="1">
+    <row r="74" spans="1:5" ht="15" hidden="1">
       <c r="A74" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="B74" s="41">
-        <v>1072.675</v>
-      </c>
-      <c r="C74" s="11">
-        <v>20</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B74" s="12">
+        <v>8150.3249999999998</v>
+      </c>
+      <c r="C74" s="11"/>
       <c r="D74" s="13">
         <f t="shared" si="0"/>
-        <v>21453.5</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>89</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E74" s="11"/>
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="11" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B75" s="12">
-        <v>1077.6875</v>
+        <v>9067.6124999999993</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="13">
@@ -2334,196 +2276,192 @@
     </row>
     <row r="76" spans="1:5" ht="15" hidden="1">
       <c r="A76" s="11" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="B76" s="12">
-        <v>1101.75</v>
+        <v>8565.36</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E76" s="11"/>
-    </row>
-    <row r="77" spans="1:5" ht="15.75" thickBot="1">
+      <c r="E76" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15" hidden="1">
       <c r="A77" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B77" s="41">
-        <v>5257.11</v>
-      </c>
-      <c r="C77" s="11">
-        <v>5</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B77" s="12">
+        <v>11854.5625</v>
+      </c>
+      <c r="C77" s="11"/>
       <c r="D77" s="13">
         <f t="shared" si="0"/>
-        <v>26285.55</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>150</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E77" s="11"/>
     </row>
     <row r="78" spans="1:5" ht="15" hidden="1">
       <c r="A78" s="11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B78" s="12">
-        <v>1303.25</v>
+        <v>10616.475</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E78" s="11"/>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1">
+      <c r="E78" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" hidden="1">
       <c r="A79" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B79" s="41">
-        <v>4252.6049999999996</v>
-      </c>
-      <c r="C79" s="11">
-        <v>10</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B79" s="12">
+        <v>12215.4625</v>
+      </c>
+      <c r="C79" s="11"/>
       <c r="D79" s="13">
         <f t="shared" si="0"/>
-        <v>42526.049999999996</v>
+        <v>0</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" hidden="1">
       <c r="A80" s="11" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="B80" s="12">
-        <v>8150.3249999999998</v>
+        <v>12691.65</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E80" s="11"/>
+      <c r="E80" s="11" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="81" spans="1:5" ht="15" hidden="1">
       <c r="A81" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B81" s="12">
-        <v>9067.6124999999993</v>
+        <v>9097.6875</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E81" s="11"/>
+      <c r="E81" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="15" hidden="1">
       <c r="A82" s="11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B82" s="12">
-        <v>8565.36</v>
+        <v>10285.65</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E82" s="14" t="s">
-        <v>84</v>
+      <c r="E82" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" hidden="1">
       <c r="A83" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B83" s="12">
-        <v>11854.5625</v>
+        <v>6342.8175000000001</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E83" s="11"/>
+      <c r="E83" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="84" spans="1:5" ht="15" hidden="1">
       <c r="A84" s="11" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="B84" s="12">
-        <v>10616.475</v>
+        <v>17443.5</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E84" s="11" t="s">
-        <v>84</v>
-      </c>
+      <c r="E84" s="11"/>
     </row>
     <row r="85" spans="1:5" ht="15" hidden="1">
       <c r="A85" s="11" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="B85" s="12">
-        <v>12215.4625</v>
+        <v>13914.7</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E85" s="11" t="s">
-        <v>89</v>
-      </c>
+      <c r="E85" s="11"/>
     </row>
     <row r="86" spans="1:5" ht="15" hidden="1">
       <c r="A86" s="11" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="B86" s="12">
-        <v>12691.65</v>
+        <v>12501.18</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>133</v>
-      </c>
+        <f t="shared" ref="D86" si="2">C86*B86</f>
+        <v>0</v>
+      </c>
+      <c r="E86" s="11"/>
     </row>
     <row r="87" spans="1:5" ht="15" hidden="1">
       <c r="A87" s="11" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="B87" s="12">
-        <v>9097.6875</v>
+        <v>23704.11</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>84</v>
-      </c>
+        <f t="shared" ref="D87" si="3">C87*B87</f>
+        <v>0</v>
+      </c>
+      <c r="E87" s="11"/>
     </row>
     <row r="88" spans="1:5" ht="15" hidden="1">
       <c r="A88" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B88" s="12">
-        <v>10285.65</v>
+        <v>1371.42</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="13">
@@ -2531,854 +2469,757 @@
         <v>0</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15" hidden="1">
       <c r="A89" s="11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B89" s="12">
-        <v>6342.8175000000001</v>
+        <v>1410.5174999999999</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E89" s="11" t="s">
-        <v>84</v>
-      </c>
+      <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:5" ht="15" hidden="1">
       <c r="A90" s="11" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="B90" s="12">
-        <v>17443.5</v>
+        <v>1694.2249999999999</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E90" s="11"/>
+        <f t="shared" ref="D90:D128" si="4">C90*B90</f>
+        <v>0</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="91" spans="1:5" ht="15" hidden="1">
       <c r="A91" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B91" s="12">
-        <v>13914.7</v>
+        <v>124</v>
+      </c>
+      <c r="B91" s="17">
+        <v>1219.04</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E91" s="11"/>
     </row>
-    <row r="92" spans="1:5" ht="15" hidden="1">
+    <row r="92" spans="1:5" ht="15">
       <c r="A92" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B92" s="12">
-        <v>12501.18</v>
-      </c>
-      <c r="C92" s="11"/>
+        <v>129</v>
+      </c>
+      <c r="B92" s="18">
+        <v>1336.33</v>
+      </c>
+      <c r="C92" s="11">
+        <v>10</v>
+      </c>
       <c r="D92" s="13">
-        <f t="shared" ref="D92" si="3">C92*B92</f>
-        <v>0</v>
-      </c>
-      <c r="E92" s="11"/>
+        <f t="shared" si="4"/>
+        <v>13363.3</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="93" spans="1:5" ht="15" hidden="1">
       <c r="A93" s="11" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="B93" s="12">
-        <v>23704.11</v>
+        <v>1871.6675</v>
       </c>
       <c r="C93" s="11"/>
       <c r="D93" s="13">
-        <f t="shared" ref="D93" si="4">C93*B93</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E93" s="11"/>
     </row>
     <row r="94" spans="1:5" ht="15" hidden="1">
       <c r="A94" s="11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B94" s="12">
-        <v>1371.42</v>
+        <v>1854.625</v>
       </c>
       <c r="C94" s="11"/>
       <c r="D94" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>84</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E94" s="11"/>
     </row>
     <row r="95" spans="1:5" ht="15" hidden="1">
       <c r="A95" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B95" s="12">
-        <v>1410.5174999999999</v>
+        <v>1446.6075000000001</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E95" s="11"/>
     </row>
     <row r="96" spans="1:5" ht="15" hidden="1">
       <c r="A96" s="11" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B96" s="12">
-        <v>1694.2249999999999</v>
+        <v>7586.92</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="13">
-        <f t="shared" ref="D96:D135" si="5">C96*B96</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" hidden="1">
       <c r="A97" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B97" s="17">
-        <v>1219.04</v>
+        <v>84</v>
+      </c>
+      <c r="B97" s="12">
+        <v>8641.5499999999993</v>
       </c>
       <c r="C97" s="11"/>
       <c r="D97" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E97" s="11"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E97" s="11" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="15" hidden="1">
       <c r="A98" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B98" s="18">
-        <v>1336.33</v>
+        <v>62</v>
+      </c>
+      <c r="B98" s="12">
+        <v>5183.9274999999998</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E98" s="11"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="99" spans="1:5" ht="15" hidden="1">
       <c r="A99" s="11" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B99" s="12">
-        <v>1871.6675</v>
+        <v>5455.6049999999996</v>
       </c>
       <c r="C99" s="11"/>
       <c r="D99" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E99" s="11"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="100" spans="1:5" ht="15" hidden="1">
       <c r="A100" s="11" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B100" s="12">
-        <v>1854.625</v>
+        <v>5510.74</v>
       </c>
       <c r="C100" s="11"/>
       <c r="D100" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E100" s="11"/>
-    </row>
-    <row r="101" spans="1:5" ht="15" hidden="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15">
       <c r="A101" s="11" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="B101" s="12">
-        <v>1446.6075000000001</v>
-      </c>
-      <c r="C101" s="11"/>
+        <v>4896.21</v>
+      </c>
+      <c r="C101" s="11">
+        <v>3</v>
+      </c>
       <c r="D101" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E101" s="11"/>
+        <f t="shared" si="4"/>
+        <v>14688.630000000001</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="102" spans="1:5" ht="15" hidden="1">
       <c r="A102" s="11" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="B102" s="12">
-        <v>7586.92</v>
+        <v>5150.8500000000004</v>
       </c>
       <c r="C102" s="11"/>
       <c r="D102" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="15" hidden="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15">
       <c r="A103" s="11" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="B103" s="12">
-        <v>8641.5499999999993</v>
-      </c>
-      <c r="C103" s="11"/>
+        <v>5310.24</v>
+      </c>
+      <c r="C103" s="11">
+        <v>5</v>
+      </c>
       <c r="D103" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>26551.199999999997</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>89</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" hidden="1">
       <c r="A104" s="11" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
       <c r="B104" s="12">
-        <v>5183.9274999999998</v>
+        <v>5423.53</v>
       </c>
       <c r="C104" s="11"/>
       <c r="D104" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" hidden="1">
       <c r="A105" s="11" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="B105" s="12">
-        <v>5455.6049999999996</v>
+        <v>5940.82</v>
       </c>
       <c r="C105" s="11"/>
       <c r="D105" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D105:D106" si="5">C105*B105</f>
         <v>0</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15" hidden="1">
       <c r="A106" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B106" s="41">
-        <v>5310.2425000000003</v>
-      </c>
-      <c r="C106" s="11">
-        <v>5</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B106" s="12">
+        <v>5257.11</v>
+      </c>
+      <c r="C106" s="11"/>
       <c r="D106" s="13">
         <f t="shared" si="5"/>
-        <v>26551.212500000001</v>
+        <v>0</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15" hidden="1">
       <c r="A107" s="11" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B107" s="12">
-        <v>5510.74</v>
-      </c>
-      <c r="C107" s="11">
-        <f>SUBTOTAL(9,C57:C106)</f>
-        <v>190</v>
-      </c>
+        <v>2900.2325000000001</v>
+      </c>
+      <c r="C107" s="11"/>
       <c r="D107" s="13">
-        <f t="shared" si="5"/>
-        <v>1047040.6</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="15" hidden="1">
       <c r="A108" s="11" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="B108" s="12">
-        <v>4896.21</v>
+        <v>3143.84</v>
       </c>
       <c r="C108" s="11"/>
       <c r="D108" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E108" s="11"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="109" spans="1:5" ht="15" hidden="1">
       <c r="A109" s="11" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="B109" s="12">
-        <v>5150.8500000000004</v>
+        <v>3518.7750000000001</v>
       </c>
       <c r="C109" s="11"/>
       <c r="D109" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E109" s="11" t="s">
-        <v>141</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E109" s="11"/>
     </row>
     <row r="110" spans="1:5" ht="15" hidden="1">
       <c r="A110" s="11" t="s">
-        <v>145</v>
+        <v>54</v>
       </c>
       <c r="B110" s="12">
-        <v>5310.24</v>
+        <v>3556.87</v>
       </c>
       <c r="C110" s="11"/>
       <c r="D110" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="15" hidden="1">
       <c r="A111" s="11" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B111" s="12">
-        <v>5423.53</v>
+        <v>3471.66</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E111" s="11" t="s">
-        <v>84</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E111" s="11"/>
     </row>
     <row r="112" spans="1:5" ht="15" hidden="1">
       <c r="A112" s="11" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="B112" s="12">
-        <v>5940.82</v>
+        <v>3919.7750000000001</v>
       </c>
       <c r="C112" s="11"/>
       <c r="D112" s="13">
-        <f t="shared" ref="D112:D113" si="6">C112*B112</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="15" hidden="1">
       <c r="A113" s="11" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="B113" s="12">
-        <v>5257.11</v>
+        <v>4534.3074999999999</v>
       </c>
       <c r="C113" s="11"/>
       <c r="D113" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="15" hidden="1">
       <c r="A114" s="11" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="B114" s="12">
-        <v>2900.2325000000001</v>
+        <v>3433.56</v>
       </c>
       <c r="C114" s="11"/>
       <c r="D114" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E114" s="11" t="s">
-        <v>84</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E114" s="11"/>
     </row>
     <row r="115" spans="1:5" ht="15" hidden="1">
       <c r="A115" s="11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B115" s="12">
-        <v>3143.84</v>
+        <v>4476.1625000000004</v>
       </c>
       <c r="C115" s="11"/>
       <c r="D115" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E115" s="11" t="s">
-        <v>89</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E115" s="11"/>
     </row>
     <row r="116" spans="1:5" ht="15" hidden="1">
       <c r="A116" s="11" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="B116" s="12">
-        <v>3518.7750000000001</v>
+        <v>4575.41</v>
       </c>
       <c r="C116" s="11"/>
       <c r="D116" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E116" s="11"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="117" spans="1:5" ht="15" hidden="1">
       <c r="A117" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B117" s="12">
-        <v>3556.87</v>
+        <v>5269.14</v>
       </c>
       <c r="C117" s="11"/>
       <c r="D117" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15" hidden="1">
       <c r="A118" s="11" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="B118" s="12">
-        <v>3471.66</v>
+        <v>5921.7674999999999</v>
       </c>
       <c r="C118" s="11"/>
       <c r="D118" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E118" s="11"/>
-    </row>
-    <row r="119" spans="1:5" ht="15" hidden="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="12" hidden="1" customHeight="1">
       <c r="A119" s="11" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B119" s="12">
-        <v>3919.7750000000001</v>
+        <v>4849.09</v>
       </c>
       <c r="C119" s="11"/>
       <c r="D119" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E119" s="11" t="s">
-        <v>84</v>
-      </c>
+        <f>C119*B119</f>
+        <v>0</v>
+      </c>
+      <c r="E119" s="11"/>
     </row>
     <row r="120" spans="1:5" ht="15" hidden="1">
       <c r="A120" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B120" s="12">
-        <v>4534.3074999999999</v>
+        <v>3934.8125</v>
       </c>
       <c r="C120" s="11"/>
       <c r="D120" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" hidden="1">
       <c r="A121" s="11" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="B121" s="12">
-        <v>3433.56</v>
+        <v>4027.0425</v>
       </c>
       <c r="C121" s="11"/>
       <c r="D121" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E121" s="11"/>
-    </row>
-    <row r="122" spans="1:5" ht="15" hidden="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15">
       <c r="A122" s="11" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="B122" s="12">
-        <v>4476.1625000000004</v>
-      </c>
-      <c r="C122" s="11"/>
+        <v>3892.71</v>
+      </c>
+      <c r="C122" s="11">
+        <v>10</v>
+      </c>
       <c r="D122" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E122" s="11"/>
+        <f t="shared" si="4"/>
+        <v>38927.1</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="123" spans="1:5" ht="15" hidden="1">
       <c r="A123" s="11" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="B123" s="12">
-        <v>4575.41</v>
+        <v>4507.24</v>
       </c>
       <c r="C123" s="11"/>
       <c r="D123" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" hidden="1">
       <c r="A124" s="11" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B124" s="12">
-        <v>5269.14</v>
+        <v>4409</v>
       </c>
       <c r="C124" s="11"/>
       <c r="D124" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="15" hidden="1">
       <c r="A125" s="11" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="B125" s="12">
-        <v>5921.7674999999999</v>
+        <v>4165.3900000000003</v>
       </c>
       <c r="C125" s="11"/>
       <c r="D125" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E125" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="12" hidden="1" customHeight="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E125" s="11"/>
+    </row>
+    <row r="126" spans="1:5" ht="15" hidden="1">
       <c r="A126" s="11" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B126" s="12">
-        <v>4849.09</v>
+        <v>4252.6099999999997</v>
       </c>
       <c r="C126" s="11"/>
       <c r="D126" s="13">
-        <f>C126*B126</f>
-        <v>0</v>
-      </c>
-      <c r="E126" s="11"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E126" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="127" spans="1:5" ht="15" hidden="1">
       <c r="A127" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B127" s="12">
-        <v>3934.8125</v>
+        <v>12741.775</v>
       </c>
       <c r="C127" s="11"/>
       <c r="D127" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E127" s="11" t="s">
-        <v>84</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E127" s="11"/>
     </row>
     <row r="128" spans="1:5" ht="15" hidden="1">
       <c r="A128" s="11" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="B128" s="12">
-        <v>4027.0425</v>
+        <v>12310.7</v>
       </c>
       <c r="C128" s="11"/>
       <c r="D128" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" ht="15" hidden="1">
-      <c r="A129" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B129" s="12">
-        <v>3892.71</v>
-      </c>
-      <c r="C129" s="11"/>
-      <c r="D129" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E129" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="15" hidden="1">
-      <c r="A130" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B130" s="12">
-        <v>4507.24</v>
-      </c>
-      <c r="C130" s="11"/>
-      <c r="D130" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E130" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="15" hidden="1">
-      <c r="A131" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B131" s="12">
-        <v>4409</v>
-      </c>
-      <c r="C131" s="11"/>
-      <c r="D131" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E131" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="15" hidden="1">
-      <c r="A132" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B132" s="12">
-        <v>4165.3900000000003</v>
-      </c>
-      <c r="C132" s="11"/>
-      <c r="D132" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E132" s="11"/>
-    </row>
-    <row r="133" spans="1:9" ht="15" hidden="1">
-      <c r="A133" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B133" s="12">
-        <v>4252.6099999999997</v>
-      </c>
-      <c r="C133" s="11"/>
-      <c r="D133" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E133" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="15" hidden="1">
-      <c r="A134" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B134" s="12">
-        <v>12741.775</v>
-      </c>
-      <c r="C134" s="11"/>
-      <c r="D134" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E134" s="11"/>
-    </row>
-    <row r="135" spans="1:9" ht="15" hidden="1">
-      <c r="A135" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B135" s="12">
-        <v>12310.7</v>
-      </c>
-      <c r="C135" s="11"/>
-      <c r="D135" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E135" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A136" s="37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" s="2" customFormat="1" ht="15">
+      <c r="A129" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B129" s="39"/>
+      <c r="C129" s="19">
+        <f>SUM(C9:C99)</f>
+        <v>75</v>
+      </c>
+      <c r="D129" s="20">
+        <f>SUM(D5:D128)</f>
+        <v>221739.93000000002</v>
+      </c>
+      <c r="E129" s="19"/>
+    </row>
+    <row r="130" spans="1:9" ht="9.75" customHeight="1">
+      <c r="A130" s="3"/>
+    </row>
+    <row r="131" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A131" s="21"/>
+      <c r="B131" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C131" s="40"/>
+      <c r="D131" s="40"/>
+      <c r="E131" s="22"/>
+    </row>
+    <row r="132" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A132" s="23"/>
+      <c r="B132" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C132" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B136" s="37"/>
-      <c r="C136" s="19">
-        <f>SUM(C57:C106)</f>
-        <v>190</v>
-      </c>
-      <c r="D136" s="20">
-        <f>SUM(D57:D106)</f>
-        <v>338123.2</v>
-      </c>
-      <c r="E136" s="19"/>
-    </row>
-    <row r="137" spans="1:9" ht="9.75" customHeight="1">
-      <c r="A137" s="3"/>
+      <c r="D132" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E132" s="22"/>
+      <c r="I132" s="25"/>
+    </row>
+    <row r="133" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A133" s="26"/>
+      <c r="B133" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C133" s="27">
+        <v>0</v>
+      </c>
+      <c r="D133" s="11"/>
+      <c r="E133" s="22"/>
+    </row>
+    <row r="134" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A134" s="26"/>
+      <c r="B134" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C134" s="32">
+        <v>220000</v>
+      </c>
+      <c r="D134" s="11"/>
+      <c r="E134" s="22"/>
+    </row>
+    <row r="135" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A135" s="26"/>
+      <c r="B135" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C135" s="27">
+        <v>0</v>
+      </c>
+      <c r="D135" s="11"/>
+      <c r="E135" s="22"/>
+    </row>
+    <row r="136" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A136" s="26"/>
+      <c r="B136" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C136" s="27"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="22"/>
+    </row>
+    <row r="137" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A137" s="26"/>
+      <c r="B137" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C137" s="27">
+        <v>0</v>
+      </c>
+      <c r="D137" s="11"/>
+      <c r="E137" s="22"/>
     </row>
     <row r="138" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A138" s="21"/>
-      <c r="B138" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C138" s="38"/>
-      <c r="D138" s="38"/>
+      <c r="A138" s="26"/>
+      <c r="B138" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C138" s="27">
+        <v>0</v>
+      </c>
+      <c r="D138" s="11"/>
       <c r="E138" s="22"/>
     </row>
     <row r="139" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A139" s="23"/>
-      <c r="B139" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C139" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D139" s="24" t="s">
+      <c r="B139" s="28" t="s">
         <v>70</v>
       </c>
+      <c r="C139" s="29">
+        <f>SUM(C133:C138)</f>
+        <v>220000</v>
+      </c>
+      <c r="D139" s="30"/>
       <c r="E139" s="22"/>
-      <c r="I139" s="25"/>
-    </row>
-    <row r="140" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A140" s="26"/>
-      <c r="B140" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C140" s="27">
-        <v>0</v>
-      </c>
-      <c r="D140" s="11"/>
-      <c r="E140" s="22"/>
-    </row>
-    <row r="141" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A141" s="26"/>
-      <c r="B141" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C141" s="42">
-        <v>150000</v>
-      </c>
-      <c r="D141" s="11"/>
-      <c r="E141" s="22"/>
-    </row>
-    <row r="142" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A142" s="26"/>
-      <c r="B142" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C142" s="27">
-        <v>0</v>
-      </c>
-      <c r="D142" s="11"/>
-      <c r="E142" s="22"/>
-    </row>
-    <row r="143" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A143" s="26"/>
-      <c r="B143" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C143" s="27"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="22"/>
-    </row>
-    <row r="144" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A144" s="26"/>
-      <c r="B144" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C144" s="27">
-        <v>0</v>
-      </c>
-      <c r="D144" s="11"/>
-      <c r="E144" s="22"/>
-    </row>
-    <row r="145" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A145" s="26"/>
-      <c r="B145" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C145" s="27">
-        <v>0</v>
-      </c>
-      <c r="D145" s="11"/>
-      <c r="E145" s="22"/>
-    </row>
-    <row r="146" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A146" s="23"/>
-      <c r="B146" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C146" s="29">
-        <f>SUM(C140:C145)</f>
-        <v>150000</v>
-      </c>
-      <c r="D146" s="30"/>
-      <c r="E146" s="22"/>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="3"/>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140" s="3"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E136">
+  <autoFilter ref="A4:E129">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3388,8 +3229,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="B131:D131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
17.04.19 Today Sales Details 08:56 PM
</commit_message>
<xml_diff>
--- a/Daily requisition analysis of Tulip -2, Bagha..xlsx
+++ b/Daily requisition analysis of Tulip -2, Bagha..xlsx
@@ -10,14 +10,14 @@
     <sheet name="Daily Requisition" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$4:$E$130</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="160">
   <si>
     <t>Model Name</t>
   </si>
@@ -490,10 +490,13 @@
     <t>BL90</t>
   </si>
   <si>
-    <t>16.04.19</t>
-  </si>
-  <si>
     <t>Yellow_Black</t>
+  </si>
+  <si>
+    <t>17.04.19</t>
+  </si>
+  <si>
+    <t>L40</t>
   </si>
 </sst>
 </file>
@@ -1131,13 +1134,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H101" sqref="H101"/>
+      <selection pane="bottomRight" activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1182,7 +1185,7 @@
         <v>79</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1227,7 +1230,7 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="13">
-        <f t="shared" ref="D6:D89" si="0">C6*B6</f>
+        <f t="shared" ref="D6:D90" si="0">C6*B6</f>
         <v>0</v>
       </c>
       <c r="E6" s="11"/>
@@ -1248,37 +1251,33 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="15" hidden="1">
       <c r="A8" s="11" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="12">
         <v>901.24749999999995</v>
       </c>
-      <c r="C8" s="11">
-        <v>20</v>
-      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="13">
         <f>SUM(B8*C8)</f>
-        <v>18024.949999999997</v>
+        <v>0</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" hidden="1">
       <c r="A9" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B9" s="12">
         <v>858.14</v>
       </c>
-      <c r="C9" s="11">
-        <v>20</v>
-      </c>
+      <c r="C9" s="11"/>
       <c r="D9" s="13">
         <f t="shared" si="0"/>
-        <v>17162.8</v>
+        <v>0</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>152</v>
@@ -1372,19 +1371,17 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="15" hidden="1">
       <c r="A16" s="11" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="12">
         <v>1238.0875000000001</v>
       </c>
-      <c r="C16" s="11">
-        <v>20</v>
-      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="13">
         <f t="shared" si="0"/>
-        <v>24761.75</v>
+        <v>0</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>87</v>
@@ -1642,19 +1639,17 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A34" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B34" s="15">
         <v>1159.8900000000001</v>
       </c>
-      <c r="C34" s="11">
-        <v>20</v>
-      </c>
+      <c r="C34" s="11"/>
       <c r="D34" s="16">
         <f t="shared" si="0"/>
-        <v>23197.800000000003</v>
+        <v>0</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>87</v>
@@ -1984,19 +1979,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15">
+    <row r="56" spans="1:5" ht="15" hidden="1">
       <c r="A56" s="11" t="s">
         <v>143</v>
       </c>
       <c r="B56" s="12">
         <v>9012.48</v>
       </c>
-      <c r="C56" s="11">
-        <v>5</v>
-      </c>
+      <c r="C56" s="11"/>
       <c r="D56" s="13">
         <f t="shared" si="0"/>
-        <v>45062.399999999994</v>
+        <v>0</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>145</v>
@@ -2190,26 +2183,30 @@
       </c>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" spans="1:5" ht="15" hidden="1">
+    <row r="70" spans="1:5" ht="15">
       <c r="A70" s="11" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="B70" s="12">
-        <v>1273.175</v>
-      </c>
-      <c r="C70" s="11"/>
+        <v>1014.53</v>
+      </c>
+      <c r="C70" s="11">
+        <v>13</v>
+      </c>
       <c r="D70" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E70" s="11"/>
+        <f>SUM(B70*C70)</f>
+        <v>13188.89</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1">
       <c r="A71" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B71" s="12">
-        <v>1077.6875</v>
+        <v>1273.175</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="13">
@@ -2220,10 +2217,10 @@
     </row>
     <row r="72" spans="1:5" ht="15" hidden="1">
       <c r="A72" s="11" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="B72" s="12">
-        <v>1101.75</v>
+        <v>1077.6875</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="13">
@@ -2234,10 +2231,10 @@
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1">
       <c r="A73" s="11" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="B73" s="12">
-        <v>1303.25</v>
+        <v>1101.75</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="13">
@@ -2248,10 +2245,10 @@
     </row>
     <row r="74" spans="1:5" ht="15" hidden="1">
       <c r="A74" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B74" s="12">
-        <v>8150.3249999999998</v>
+        <v>1303.25</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="13">
@@ -2262,10 +2259,10 @@
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1">
       <c r="A75" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B75" s="12">
-        <v>9067.6124999999993</v>
+        <v>8150.3249999999998</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="13">
@@ -2276,56 +2273,54 @@
     </row>
     <row r="76" spans="1:5" ht="15" hidden="1">
       <c r="A76" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B76" s="12">
-        <v>8565.36</v>
+        <v>9067.6124999999993</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E76" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="E76" s="11"/>
     </row>
     <row r="77" spans="1:5" ht="15" hidden="1">
       <c r="A77" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B77" s="12">
-        <v>11854.5625</v>
+        <v>8565.36</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E77" s="11"/>
+      <c r="E77" s="14" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="78" spans="1:5" ht="15" hidden="1">
       <c r="A78" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B78" s="12">
-        <v>10616.475</v>
+        <v>11854.5625</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E78" s="11" t="s">
-        <v>82</v>
-      </c>
+      <c r="E78" s="11"/>
     </row>
     <row r="79" spans="1:5" ht="15" hidden="1">
       <c r="A79" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B79" s="12">
-        <v>12215.4625</v>
+        <v>10616.475</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="13">
@@ -2333,15 +2328,15 @@
         <v>0</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" hidden="1">
       <c r="A80" s="11" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="B80" s="12">
-        <v>12691.65</v>
+        <v>12215.4625</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="13">
@@ -2349,15 +2344,15 @@
         <v>0</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" hidden="1">
       <c r="A81" s="11" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B81" s="12">
-        <v>9097.6875</v>
+        <v>12691.65</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="13">
@@ -2365,15 +2360,15 @@
         <v>0</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" hidden="1">
       <c r="A82" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B82" s="12">
-        <v>10285.65</v>
+        <v>9097.6875</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="13">
@@ -2386,10 +2381,10 @@
     </row>
     <row r="83" spans="1:5" ht="15" hidden="1">
       <c r="A83" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B83" s="12">
-        <v>6342.8175000000001</v>
+        <v>10285.65</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="13">
@@ -2402,24 +2397,26 @@
     </row>
     <row r="84" spans="1:5" ht="15" hidden="1">
       <c r="A84" s="11" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="B84" s="12">
-        <v>17443.5</v>
+        <v>6342.8175000000001</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E84" s="11"/>
+      <c r="E84" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="85" spans="1:5" ht="15" hidden="1">
       <c r="A85" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B85" s="12">
-        <v>13914.7</v>
+        <v>17443.5</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="13">
@@ -2430,130 +2427,128 @@
     </row>
     <row r="86" spans="1:5" ht="15" hidden="1">
       <c r="A86" s="11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B86" s="12">
-        <v>12501.18</v>
+        <v>13914.7</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="13">
-        <f t="shared" ref="D86" si="2">C86*B86</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E86" s="11"/>
     </row>
     <row r="87" spans="1:5" ht="15" hidden="1">
       <c r="A87" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B87" s="12">
-        <v>23704.11</v>
+        <v>12501.18</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="13">
-        <f t="shared" ref="D87" si="3">C87*B87</f>
+        <f t="shared" ref="D87" si="2">C87*B87</f>
         <v>0</v>
       </c>
       <c r="E87" s="11"/>
     </row>
     <row r="88" spans="1:5" ht="15" hidden="1">
       <c r="A88" s="11" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="B88" s="12">
-        <v>1371.42</v>
+        <v>23704.11</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>82</v>
-      </c>
+        <f t="shared" ref="D88" si="3">C88*B88</f>
+        <v>0</v>
+      </c>
+      <c r="E88" s="11"/>
     </row>
     <row r="89" spans="1:5" ht="15" hidden="1">
       <c r="A89" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B89" s="12">
-        <v>1410.5174999999999</v>
+        <v>1371.42</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E89" s="11"/>
+      <c r="E89" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="15" hidden="1">
       <c r="A90" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B90" s="12">
-        <v>1694.2249999999999</v>
+        <v>1410.5174999999999</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="13">
-        <f t="shared" ref="D90:D128" si="4">C90*B90</f>
-        <v>0</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>82</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E90" s="11"/>
     </row>
     <row r="91" spans="1:5" ht="15" hidden="1">
       <c r="A91" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B91" s="17">
-        <v>1219.04</v>
+        <v>48</v>
+      </c>
+      <c r="B91" s="12">
+        <v>1694.2249999999999</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E91" s="11"/>
-    </row>
-    <row r="92" spans="1:5" ht="15">
+        <f t="shared" ref="D91:D129" si="4">C91*B91</f>
+        <v>0</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15" hidden="1">
       <c r="A92" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B92" s="18">
-        <v>1336.33</v>
-      </c>
-      <c r="C92" s="11">
-        <v>10</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B92" s="17">
+        <v>1219.04</v>
+      </c>
+      <c r="C92" s="11"/>
       <c r="D92" s="13">
         <f t="shared" si="4"/>
-        <v>13363.3</v>
-      </c>
-      <c r="E92" s="11" t="s">
-        <v>87</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" ht="15" hidden="1">
       <c r="A93" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B93" s="12">
-        <v>1871.6675</v>
+        <v>129</v>
+      </c>
+      <c r="B93" s="18">
+        <v>1336.33</v>
       </c>
       <c r="C93" s="11"/>
       <c r="D93" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E93" s="11"/>
+      <c r="E93" s="11" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="94" spans="1:5" ht="15" hidden="1">
       <c r="A94" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B94" s="12">
-        <v>1854.625</v>
+        <v>1871.6675</v>
       </c>
       <c r="C94" s="11"/>
       <c r="D94" s="13">
@@ -2564,10 +2559,10 @@
     </row>
     <row r="95" spans="1:5" ht="15" hidden="1">
       <c r="A95" s="11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B95" s="12">
-        <v>1446.6075000000001</v>
+        <v>1854.625</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="13">
@@ -2578,26 +2573,24 @@
     </row>
     <row r="96" spans="1:5" ht="15" hidden="1">
       <c r="A96" s="11" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="B96" s="12">
-        <v>7586.92</v>
+        <v>1446.6075000000001</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E96" s="11" t="s">
-        <v>87</v>
-      </c>
+      <c r="E96" s="11"/>
     </row>
     <row r="97" spans="1:5" ht="15" hidden="1">
       <c r="A97" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B97" s="12">
-        <v>8641.5499999999993</v>
+        <v>7586.92</v>
       </c>
       <c r="C97" s="11"/>
       <c r="D97" s="13">
@@ -2610,10 +2603,10 @@
     </row>
     <row r="98" spans="1:5" ht="15" hidden="1">
       <c r="A98" s="11" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B98" s="12">
-        <v>5183.9274999999998</v>
+        <v>8641.5499999999993</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="13">
@@ -2621,15 +2614,15 @@
         <v>0</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" hidden="1">
       <c r="A99" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B99" s="12">
-        <v>5455.6049999999996</v>
+        <v>5183.9274999999998</v>
       </c>
       <c r="C99" s="11"/>
       <c r="D99" s="13">
@@ -2642,10 +2635,10 @@
     </row>
     <row r="100" spans="1:5" ht="15" hidden="1">
       <c r="A100" s="11" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="B100" s="12">
-        <v>5510.74</v>
+        <v>5455.6049999999996</v>
       </c>
       <c r="C100" s="11"/>
       <c r="D100" s="13">
@@ -2656,19 +2649,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15">
+    <row r="101" spans="1:5" ht="15" hidden="1">
       <c r="A101" s="11" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B101" s="12">
-        <v>4896.21</v>
-      </c>
-      <c r="C101" s="11">
-        <v>3</v>
-      </c>
+        <v>5510.74</v>
+      </c>
+      <c r="C101" s="11"/>
       <c r="D101" s="13">
         <f t="shared" si="4"/>
-        <v>14688.630000000001</v>
+        <v>0</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>82</v>
@@ -2676,10 +2667,10 @@
     </row>
     <row r="102" spans="1:5" ht="15" hidden="1">
       <c r="A102" s="11" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B102" s="12">
-        <v>5150.8500000000004</v>
+        <v>4896.21</v>
       </c>
       <c r="C102" s="11"/>
       <c r="D102" s="13">
@@ -2687,53 +2678,53 @@
         <v>0</v>
       </c>
       <c r="E102" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15" hidden="1">
+      <c r="A103" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" s="12">
+        <v>5150.8500000000004</v>
+      </c>
+      <c r="C103" s="11"/>
+      <c r="D103" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E103" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15">
-      <c r="A103" s="11" t="s">
+    <row r="104" spans="1:5" ht="15">
+      <c r="A104" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B103" s="12">
+      <c r="B104" s="12">
         <v>5310.24</v>
       </c>
-      <c r="C103" s="11">
-        <v>5</v>
-      </c>
-      <c r="D103" s="13">
-        <f t="shared" si="4"/>
-        <v>26551.199999999997</v>
-      </c>
-      <c r="E103" s="11" t="s">
+      <c r="C104" s="11">
+        <v>3</v>
+      </c>
+      <c r="D104" s="13">
+        <f t="shared" si="4"/>
+        <v>15930.72</v>
+      </c>
+      <c r="E104" s="11" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="15" hidden="1">
-      <c r="A104" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B104" s="12">
-        <v>5423.53</v>
-      </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E104" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" hidden="1">
       <c r="A105" s="11" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B105" s="12">
-        <v>5940.82</v>
+        <v>5423.53</v>
       </c>
       <c r="C105" s="11"/>
       <c r="D105" s="13">
-        <f t="shared" ref="D105:D106" si="5">C105*B105</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E105" s="11" t="s">
@@ -2742,14 +2733,14 @@
     </row>
     <row r="106" spans="1:5" ht="15" hidden="1">
       <c r="A106" s="11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B106" s="12">
-        <v>5257.11</v>
+        <v>5940.82</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D106:D107" si="5">C106*B106</f>
         <v>0</v>
       </c>
       <c r="E106" s="11" t="s">
@@ -2758,14 +2749,14 @@
     </row>
     <row r="107" spans="1:5" ht="15" hidden="1">
       <c r="A107" s="11" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="B107" s="12">
-        <v>2900.2325000000001</v>
+        <v>5257.11</v>
       </c>
       <c r="C107" s="11"/>
       <c r="D107" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E107" s="11" t="s">
@@ -2774,10 +2765,10 @@
     </row>
     <row r="108" spans="1:5" ht="15" hidden="1">
       <c r="A108" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B108" s="12">
-        <v>3143.84</v>
+        <v>2900.2325000000001</v>
       </c>
       <c r="C108" s="11"/>
       <c r="D108" s="13">
@@ -2785,75 +2776,79 @@
         <v>0</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" hidden="1">
       <c r="A109" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B109" s="12">
-        <v>3518.7750000000001</v>
+        <v>3143.84</v>
       </c>
       <c r="C109" s="11"/>
       <c r="D109" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E109" s="11"/>
+      <c r="E109" s="11" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="110" spans="1:5" ht="15" hidden="1">
       <c r="A110" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B110" s="12">
-        <v>3556.87</v>
+        <v>3518.7750000000001</v>
       </c>
       <c r="C110" s="11"/>
       <c r="D110" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E110" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="E110" s="11"/>
     </row>
     <row r="111" spans="1:5" ht="15" hidden="1">
       <c r="A111" s="11" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="B111" s="12">
-        <v>3471.66</v>
+        <v>3556.87</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E111" s="11"/>
-    </row>
-    <row r="112" spans="1:5" ht="15" hidden="1">
+      <c r="E111" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15">
       <c r="A112" s="11" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="B112" s="12">
-        <v>3919.7750000000001</v>
-      </c>
-      <c r="C112" s="11"/>
+        <v>3471.66</v>
+      </c>
+      <c r="C112" s="11">
+        <v>2</v>
+      </c>
       <c r="D112" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6943.32</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="15" hidden="1">
       <c r="A113" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B113" s="12">
-        <v>4534.3074999999999</v>
+        <v>3919.7750000000001</v>
       </c>
       <c r="C113" s="11"/>
       <c r="D113" s="13">
@@ -2866,24 +2861,26 @@
     </row>
     <row r="114" spans="1:5" ht="15" hidden="1">
       <c r="A114" s="11" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="B114" s="12">
-        <v>3433.56</v>
+        <v>4534.3074999999999</v>
       </c>
       <c r="C114" s="11"/>
       <c r="D114" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E114" s="11"/>
+      <c r="E114" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="115" spans="1:5" ht="15" hidden="1">
       <c r="A115" s="11" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="B115" s="12">
-        <v>4476.1625000000004</v>
+        <v>3433.56</v>
       </c>
       <c r="C115" s="11"/>
       <c r="D115" s="13">
@@ -2894,26 +2891,24 @@
     </row>
     <row r="116" spans="1:5" ht="15" hidden="1">
       <c r="A116" s="11" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="B116" s="12">
-        <v>4575.41</v>
+        <v>4476.1625000000004</v>
       </c>
       <c r="C116" s="11"/>
       <c r="D116" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E116" s="11" t="s">
-        <v>82</v>
-      </c>
+      <c r="E116" s="11"/>
     </row>
     <row r="117" spans="1:5" ht="15" hidden="1">
       <c r="A117" s="11" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="B117" s="12">
-        <v>5269.14</v>
+        <v>4575.41</v>
       </c>
       <c r="C117" s="11"/>
       <c r="D117" s="13">
@@ -2926,10 +2921,10 @@
     </row>
     <row r="118" spans="1:5" ht="15" hidden="1">
       <c r="A118" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B118" s="12">
-        <v>5921.7674999999999</v>
+        <v>5269.14</v>
       </c>
       <c r="C118" s="11"/>
       <c r="D118" s="13">
@@ -2940,42 +2935,42 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="12" hidden="1" customHeight="1">
+    <row r="119" spans="1:5" ht="15" hidden="1">
       <c r="A119" s="11" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="B119" s="12">
-        <v>4849.09</v>
+        <v>5921.7674999999999</v>
       </c>
       <c r="C119" s="11"/>
       <c r="D119" s="13">
-        <f>C119*B119</f>
-        <v>0</v>
-      </c>
-      <c r="E119" s="11"/>
-    </row>
-    <row r="120" spans="1:5" ht="15" hidden="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="12" hidden="1" customHeight="1">
       <c r="A120" s="11" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="B120" s="12">
-        <v>3934.8125</v>
+        <v>4849.09</v>
       </c>
       <c r="C120" s="11"/>
       <c r="D120" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>82</v>
-      </c>
+        <f>C120*B120</f>
+        <v>0</v>
+      </c>
+      <c r="E120" s="11"/>
     </row>
     <row r="121" spans="1:5" ht="15" hidden="1">
       <c r="A121" s="11" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="B121" s="12">
-        <v>4027.0425</v>
+        <v>3934.8125</v>
       </c>
       <c r="C121" s="11"/>
       <c r="D121" s="13">
@@ -2986,30 +2981,28 @@
         <v>82</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="15">
+    <row r="122" spans="1:5" ht="15" hidden="1">
       <c r="A122" s="11" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B122" s="12">
-        <v>3892.71</v>
-      </c>
-      <c r="C122" s="11">
-        <v>10</v>
-      </c>
+        <v>4027.0425</v>
+      </c>
+      <c r="C122" s="11"/>
       <c r="D122" s="13">
         <f t="shared" si="4"/>
-        <v>38927.1</v>
+        <v>0</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>145</v>
+        <v>82</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="15" hidden="1">
       <c r="A123" s="11" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="B123" s="12">
-        <v>4507.24</v>
+        <v>3892.71</v>
       </c>
       <c r="C123" s="11"/>
       <c r="D123" s="13">
@@ -3017,15 +3010,15 @@
         <v>0</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" hidden="1">
       <c r="A124" s="11" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="B124" s="12">
-        <v>4409</v>
+        <v>4507.24</v>
       </c>
       <c r="C124" s="11"/>
       <c r="D124" s="13">
@@ -3038,123 +3031,132 @@
     </row>
     <row r="125" spans="1:5" ht="15" hidden="1">
       <c r="A125" s="11" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="B125" s="12">
-        <v>4165.3900000000003</v>
+        <v>4409</v>
       </c>
       <c r="C125" s="11"/>
       <c r="D125" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E125" s="11"/>
-    </row>
-    <row r="126" spans="1:5" ht="15" hidden="1">
+      <c r="E125" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15">
       <c r="A126" s="11" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B126" s="12">
-        <v>4252.6099999999997</v>
-      </c>
-      <c r="C126" s="11"/>
+        <v>4165.3900000000003</v>
+      </c>
+      <c r="C126" s="11">
+        <v>2</v>
+      </c>
       <c r="D126" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8330.7800000000007</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="15" hidden="1">
       <c r="A127" s="11" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="B127" s="12">
-        <v>12741.775</v>
+        <v>4252.6099999999997</v>
       </c>
       <c r="C127" s="11"/>
       <c r="D127" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E127" s="11"/>
+      <c r="E127" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="128" spans="1:5" ht="15" hidden="1">
       <c r="A128" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B128" s="12">
-        <v>12310.7</v>
+        <v>12741.775</v>
       </c>
       <c r="C128" s="11"/>
       <c r="D128" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E128" s="11" t="s">
+      <c r="E128" s="11"/>
+    </row>
+    <row r="129" spans="1:9" ht="15" hidden="1">
+      <c r="A129" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B129" s="12">
+        <v>12310.7</v>
+      </c>
+      <c r="C129" s="11"/>
+      <c r="D129" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E129" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="129" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A129" s="39" t="s">
+    <row r="130" spans="1:9" s="2" customFormat="1" ht="15">
+      <c r="A130" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B129" s="39"/>
-      <c r="C129" s="19">
-        <f>SUM(C9:C99)</f>
-        <v>75</v>
-      </c>
-      <c r="D129" s="20">
-        <f>SUM(D5:D128)</f>
-        <v>221739.93000000002</v>
-      </c>
-      <c r="E129" s="19"/>
-    </row>
-    <row r="130" spans="1:9" ht="9.75" customHeight="1">
-      <c r="A130" s="3"/>
-    </row>
-    <row r="131" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A131" s="21"/>
-      <c r="B131" s="40" t="s">
+      <c r="B130" s="39"/>
+      <c r="C130" s="19">
+        <f>SUBTOTAL(9,C70:C129)</f>
+        <v>20</v>
+      </c>
+      <c r="D130" s="20">
+        <f>SUM(D5:D129)</f>
+        <v>44393.71</v>
+      </c>
+      <c r="E130" s="19"/>
+    </row>
+    <row r="131" spans="1:9" ht="9.75" customHeight="1">
+      <c r="A131" s="3"/>
+    </row>
+    <row r="132" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A132" s="21"/>
+      <c r="B132" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C131" s="40"/>
-      <c r="D131" s="40"/>
-      <c r="E131" s="22"/>
-    </row>
-    <row r="132" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A132" s="23"/>
-      <c r="B132" s="24" t="s">
+      <c r="C132" s="40"/>
+      <c r="D132" s="40"/>
+      <c r="E132" s="22"/>
+    </row>
+    <row r="133" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A133" s="23"/>
+      <c r="B133" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C132" s="24" t="s">
+      <c r="C133" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D132" s="24" t="s">
+      <c r="D133" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E132" s="22"/>
-      <c r="I132" s="25"/>
-    </row>
-    <row r="133" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A133" s="26"/>
-      <c r="B133" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C133" s="27">
-        <v>0</v>
-      </c>
-      <c r="D133" s="11"/>
       <c r="E133" s="22"/>
+      <c r="I133" s="25"/>
     </row>
     <row r="134" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A134" s="26"/>
       <c r="B134" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C134" s="32">
-        <v>220000</v>
+        <v>73</v>
+      </c>
+      <c r="C134" s="27">
+        <v>0</v>
       </c>
       <c r="D134" s="11"/>
       <c r="E134" s="22"/>
@@ -3164,8 +3166,8 @@
       <c r="B135" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C135" s="27">
-        <v>0</v>
+      <c r="C135" s="32">
+        <v>45000</v>
       </c>
       <c r="D135" s="11"/>
       <c r="E135" s="22"/>
@@ -3173,27 +3175,27 @@
     <row r="136" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A136" s="26"/>
       <c r="B136" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C136" s="27"/>
+        <v>74</v>
+      </c>
+      <c r="C136" s="27">
+        <v>0</v>
+      </c>
       <c r="D136" s="11"/>
       <c r="E136" s="22"/>
     </row>
     <row r="137" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A137" s="26"/>
       <c r="B137" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C137" s="27">
-        <v>0</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C137" s="27"/>
       <c r="D137" s="11"/>
       <c r="E137" s="22"/>
     </row>
     <row r="138" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A138" s="26"/>
       <c r="B138" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C138" s="27">
         <v>0</v>
@@ -3202,24 +3204,35 @@
       <c r="E138" s="22"/>
     </row>
     <row r="139" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A139" s="23"/>
-      <c r="B139" s="28" t="s">
+      <c r="A139" s="26"/>
+      <c r="B139" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C139" s="27">
+        <v>0</v>
+      </c>
+      <c r="D139" s="11"/>
+      <c r="E139" s="22"/>
+    </row>
+    <row r="140" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A140" s="23"/>
+      <c r="B140" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C139" s="29">
-        <f>SUM(C133:C138)</f>
-        <v>220000</v>
-      </c>
-      <c r="D139" s="30"/>
-      <c r="E139" s="22"/>
-    </row>
-    <row r="140" spans="1:9">
-      <c r="A140" s="3"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
+      <c r="C140" s="29">
+        <f>SUM(C134:C139)</f>
+        <v>45000</v>
+      </c>
+      <c r="D140" s="30"/>
+      <c r="E140" s="22"/>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" s="3"/>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E129">
+  <autoFilter ref="A4:E130">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3229,8 +3242,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="B131:D131"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="B132:D132"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>